<commit_message>
updated price and hardware
</commit_message>
<xml_diff>
--- a/hardware component_Price List.xlsx
+++ b/hardware component_Price List.xlsx
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>